<commit_message>
add new certificate of completion of Git and Github bootcamp
</commit_message>
<xml_diff>
--- a/my_certificates.xlsx
+++ b/my_certificates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Acoptex/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Acoptex/Documents/Certificates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3DA3B7-EADF-8143-AB46-26C7F00090A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B442C29-7A97-C04E-8F9D-57A402638FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="4220" windowWidth="25440" windowHeight="14640" xr2:uid="{37EDD2C8-83CF-5C42-BE81-87BD89CCFC84}"/>
+    <workbookView xWindow="6480" yWindow="2780" windowWidth="25440" windowHeight="14620" xr2:uid="{37EDD2C8-83CF-5C42-BE81-87BD89CCFC84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Certificates</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>2023.08.08</t>
+  </si>
+  <si>
+    <t>2023.10.21</t>
+  </si>
+  <si>
+    <t>UC-e26431f6-ca7b-4eb2-827b-9f42a8cd8399</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,8 +655,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
add new certificate Git
</commit_message>
<xml_diff>
--- a/my_certificates.xlsx
+++ b/my_certificates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Acoptex/Documents/Certificates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Acoptex/Documents/My-certificates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D7EF8C-D8A0-8F4A-B3A4-42BD3106799A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5187265D-C93D-904B-B04E-81A2094EDBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="25440" windowHeight="14620" xr2:uid="{37EDD2C8-83CF-5C42-BE81-87BD89CCFC84}"/>
+    <workbookView xWindow="10140" yWindow="500" windowWidth="25440" windowHeight="14600" xr2:uid="{37EDD2C8-83CF-5C42-BE81-87BD89CCFC84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Certificates</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Git from A to Z</t>
+  </si>
+  <si>
+    <t>0898840</t>
+  </si>
+  <si>
+    <t>2020.07.05</t>
+  </si>
+  <si>
+    <t>Git</t>
   </si>
 </sst>
 </file>
@@ -550,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606EBDEE-86E8-A446-AA7E-65AB1F0A80C7}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,61 +624,61 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -677,37 +686,41 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
@@ -717,7 +730,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
@@ -727,7 +740,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
@@ -737,7 +750,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
@@ -747,7 +760,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
@@ -756,8 +769,12 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
@@ -765,45 +782,51 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2545251</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2545260</v>
+        <v>2545251</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2545260</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>